<commit_message>
done sql generation script
</commit_message>
<xml_diff>
--- a/excel/Inventory_20150416.xlsx
+++ b/excel/Inventory_20150416.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
   <si>
     <t>3000041389</t>
   </si>
@@ -98,6 +98,18 @@
   </si>
   <si>
     <t>01A011</t>
+  </si>
+  <si>
+    <t>01A012</t>
+  </si>
+  <si>
+    <t>01A013</t>
+  </si>
+  <si>
+    <t>01A014</t>
+  </si>
+  <si>
+    <t>01A015</t>
   </si>
 </sst>
 </file>
@@ -496,7 +508,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="124" zoomScaleNormal="124" zoomScalePageLayoutView="124" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -573,7 +585,7 @@
         <v>18</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G3" s="3">
         <v>3</v>
@@ -596,7 +608,7 @@
         <v>18</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="G4" s="3">
         <v>68</v>
@@ -619,7 +631,7 @@
         <v>18</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="G5" s="3">
         <v>98</v>
@@ -642,7 +654,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="G6" s="3">
         <v>20</v>

</xml_diff>

<commit_message>
fixed to update date to created_at
</commit_message>
<xml_diff>
--- a/excel/Inventory_20150416.xlsx
+++ b/excel/Inventory_20150416.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
   <si>
     <t>3000041389</t>
   </si>
@@ -107,6 +107,9 @@
   </si>
   <si>
     <t>01A015</t>
+  </si>
+  <si>
+    <t>01A011</t>
   </si>
 </sst>
 </file>
@@ -505,7 +508,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="124" zoomScaleNormal="124" zoomScalePageLayoutView="124" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -559,7 +562,7 @@
         <v>18</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="G2" s="3">
         <v>1</v>

</xml_diff>

<commit_message>
fixed script to add newline in log files
</commit_message>
<xml_diff>
--- a/excel/Inventory_20150416.xlsx
+++ b/excel/Inventory_20150416.xlsx
@@ -97,9 +97,6 @@
     <t>Surface RT 64 GB   ()</t>
   </si>
   <si>
-    <t>01A012</t>
-  </si>
-  <si>
     <t>01A013</t>
   </si>
   <si>
@@ -110,6 +107,9 @@
   </si>
   <si>
     <t>01A011</t>
+  </si>
+  <si>
+    <t>01A000</t>
   </si>
 </sst>
 </file>
@@ -508,7 +508,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="124" zoomScaleNormal="124" zoomScalePageLayoutView="124" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -562,7 +562,7 @@
         <v>18</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G2" s="3">
         <v>1</v>
@@ -585,7 +585,7 @@
         <v>18</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="G3" s="3">
         <v>3</v>
@@ -608,7 +608,7 @@
         <v>18</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G4" s="3">
         <v>68</v>
@@ -631,7 +631,7 @@
         <v>18</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G5" s="3">
         <v>98</v>
@@ -654,7 +654,7 @@
         <v>18</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="G6" s="3">
         <v>20</v>

</xml_diff>

<commit_message>
fixed to generate log file as csv
</commit_message>
<xml_diff>
--- a/excel/Inventory_20150416.xlsx
+++ b/excel/Inventory_20150416.xlsx
@@ -34,15 +34,9 @@
     <t>เครื่องถอนขนถนอมผิว EMJOI LIGHT</t>
   </si>
   <si>
-    <t>3000040851</t>
-  </si>
-  <si>
     <t>แบตเตอรี่สำรอง iWish Power Bank A5 2600 mAh Pink</t>
   </si>
   <si>
-    <t>3000038608</t>
-  </si>
-  <si>
     <t>เมาท์ไร้สาย Anitech T-632 White</t>
   </si>
   <si>
@@ -110,6 +104,12 @@
   </si>
   <si>
     <t>01A000</t>
+  </si>
+  <si>
+    <t>5000038608</t>
+  </si>
+  <si>
+    <t>5000040851</t>
   </si>
 </sst>
 </file>
@@ -508,7 +508,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="124" zoomScaleNormal="124" zoomScalePageLayoutView="124" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -524,45 +524,45 @@
   <sheetData>
     <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>22</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="G2" s="3">
         <v>1</v>
@@ -570,22 +570,22 @@
     </row>
     <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="F3" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G3" s="3">
         <v>3</v>
@@ -593,22 +593,22 @@
     </row>
     <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B4" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>18</v>
-      </c>
       <c r="F4" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="G4" s="3">
         <v>68</v>
@@ -616,22 +616,22 @@
     </row>
     <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D5" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>3</v>
-      </c>
       <c r="E5" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G5" s="3">
         <v>98</v>
@@ -639,10 +639,10 @@
     </row>
     <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C6" s="2" t="s">
         <v>0</v>
@@ -651,10 +651,10 @@
         <v>1</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="G6" s="3">
         <v>20</v>

</xml_diff>

<commit_message>
fixed to log duplicate not found location
</commit_message>
<xml_diff>
--- a/excel/Inventory_20150416.xlsx
+++ b/excel/Inventory_20150416.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
   <si>
     <t>3000041389</t>
   </si>
@@ -98,9 +98,6 @@
   </si>
   <si>
     <t>01A015</t>
-  </si>
-  <si>
-    <t>01A011</t>
   </si>
   <si>
     <t>01A000</t>
@@ -508,7 +505,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="124" zoomScaleNormal="124" zoomScalePageLayoutView="124" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -599,7 +596,7 @@
         <v>15</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D4" s="2" t="s">
         <v>3</v>
@@ -622,7 +619,7 @@
         <v>15</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D5" s="2" t="s">
         <v>2</v>
@@ -654,7 +651,7 @@
         <v>16</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G6" s="3">
         <v>20</v>

</xml_diff>

<commit_message>
fixed generate uid logic to lowercase
</commit_message>
<xml_diff>
--- a/excel/Inventory_20150416.xlsx
+++ b/excel/Inventory_20150416.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="25711"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="25908"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14560"/>
   </bookViews>
   <sheets>
-    <sheet name="Inventory for check stock" sheetId="1" r:id="rId1"/>
+    <sheet name="Inventory Repair" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -26,28 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="27">
-  <si>
-    <t>3000041389</t>
-  </si>
-  <si>
-    <t>เครื่องถอนขนถนอมผิว EMJOI LIGHT</t>
-  </si>
-  <si>
-    <t>แบตเตอรี่สำรอง iWish Power Bank A5 2600 mAh Pink</t>
-  </si>
-  <si>
-    <t>เมาท์ไร้สาย Anitech T-632 White</t>
-  </si>
-  <si>
-    <t>20150327</t>
-  </si>
-  <si>
-    <t>3000033040</t>
-  </si>
-  <si>
-    <t>Power Bank Golf LCD USB 2 Port 10400 mAh รุ่น GF-LCD04 White  White ()</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="24">
   <si>
     <t>Receiving Date (Valid for FIFO Control)</t>
   </si>
@@ -70,43 +49,55 @@
     <t>Qty On Hand</t>
   </si>
   <si>
-    <t>20150201</t>
-  </si>
-  <si>
     <t>GOOD</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>20150317</t>
-  </si>
-  <si>
-    <t>20150401</t>
-  </si>
-  <si>
-    <t>3000022118</t>
-  </si>
-  <si>
-    <t>Surface RT 64 GB   ()</t>
-  </si>
-  <si>
-    <t>01A013</t>
-  </si>
-  <si>
-    <t>01A014</t>
-  </si>
-  <si>
-    <t>01A015</t>
-  </si>
-  <si>
-    <t>01A000</t>
-  </si>
-  <si>
-    <t>5000038608</t>
-  </si>
-  <si>
-    <t>5000040851</t>
+    <t>okamoto zero zero Three 003 แพค12กล่อง</t>
+  </si>
+  <si>
+    <t>okamoto Suprema Lite แพค12กล่อง</t>
+  </si>
+  <si>
+    <t>okamoto Gel Plus แพค12กล่อง</t>
+  </si>
+  <si>
+    <t>okamoto Dot De Cool แพค12กล่อง</t>
+  </si>
+  <si>
+    <t>okamoto XL แพค12กล่อง</t>
+  </si>
+  <si>
+    <t>okamoto 003 Aloe แพค12กล่อง</t>
+  </si>
+  <si>
+    <t>okamoto Strawberry แพค12 กล่อง</t>
+  </si>
+  <si>
+    <t>okamoto Lite แพค 12 กล่อง</t>
+  </si>
+  <si>
+    <t>okamoto zero zero Three 003 แพค1กล่อง</t>
+  </si>
+  <si>
+    <t>okamoto Suprema Lite แพค1กล่อง</t>
+  </si>
+  <si>
+    <t>okamoto Gel Plus แพค1กล่อง</t>
+  </si>
+  <si>
+    <t>20150519</t>
+  </si>
+  <si>
+    <t>Supplier</t>
+  </si>
+  <si>
+    <t>LOC-1132</t>
+  </si>
+  <si>
+    <t>HAYASHI PRODUCTS CO., LTD.</t>
   </si>
 </sst>
 </file>
@@ -163,9 +154,7 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -502,159 +491,317 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" zoomScale="124" zoomScaleNormal="124" zoomScalePageLayoutView="124" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" showRuler="0" topLeftCell="D1" zoomScale="124" zoomScaleNormal="124" zoomScalePageLayoutView="124" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="33.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="65" customWidth="1"/>
-    <col min="5" max="5" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="33.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="65" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="29.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="3">
+        <v>3000041863</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="F2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="3">
+        <v>12</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3">
+        <v>3000041866</v>
+      </c>
+      <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="3">
+        <v>12</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" s="3">
+        <v>3000041869</v>
+      </c>
+      <c r="D4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="E4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="3">
         <v>12</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H4" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="3">
+        <v>3000041962</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G5" s="3">
+        <v>12</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="3">
+        <v>3000041965</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.15">
-      <c r="A2" s="2" t="s">
+      <c r="E6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G6" s="3">
+        <v>12</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="3">
+        <v>3000041968</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="3">
+        <v>12</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="3">
+        <v>3000041971</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G8" s="3">
+        <v>12</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="3">
+        <v>3000041974</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G9" s="3">
+        <v>12</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="3">
+        <v>3000041864</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G10" s="3">
+        <v>616</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C11" s="3">
+        <v>3000041867</v>
+      </c>
+      <c r="D11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C2" s="2" t="s">
+      <c r="F11" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G11" s="3">
+        <v>110</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12" s="3">
+        <v>3000041870</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G2" s="3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.15">
-      <c r="A3" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.15">
-      <c r="A4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="G4" s="3">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.15">
-      <c r="A5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="G5" s="3">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.15">
-      <c r="A6" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="G6" s="3">
-        <v>20</v>
+      <c r="F12" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G12" s="3">
+        <v>141</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>